<commit_message>
excel erweitert um datensatz photo2monet
</commit_message>
<xml_diff>
--- a/Final_Project/Material_for_Documentation/Components of the Generator loss.xlsx
+++ b/Final_Project/Material_for_Documentation/Components of the Generator loss.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fabian\Desktop\Cognitive Computing Studium\Courses first semester\Implementing ANNs with TensorFlow\IANN_group30\Final_Project\Sources_And_Material\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7febc520ade5fca9/Master_Cognitive_Computing/1_Semester/IANN_group30/Final_project/Material_for_Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F39A294-4FFD-4FF0-BCE3-4B29BB57511E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="705" yWindow="705" windowWidth="16875" windowHeight="10523" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -218,7 +218,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="de-DE"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1090,7 +1090,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="de-DE"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1125,7 +1125,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1418985760"/>
@@ -1212,7 +1212,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="de-DE"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1247,7 +1247,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1419001984"/>
@@ -1298,7 +1298,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="de-DE"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1332,7 +1332,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="de-DE"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2243,26 +2243,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
       <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.53125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.796875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.53125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.46484375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B1" s="2"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -2282,7 +2282,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="1">
         <v>150</v>
       </c>
@@ -2302,7 +2302,7 @@
         <v>0.5791309</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" s="1">
         <v>300</v>
       </c>
@@ -2322,7 +2322,7 @@
         <v>0.49004456000000002</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" s="1">
         <v>450</v>
       </c>
@@ -2342,7 +2342,7 @@
         <v>0.45827784999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" s="1">
         <v>600</v>
       </c>
@@ -2362,7 +2362,7 @@
         <v>0.44495289999999998</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" s="1">
         <v>750</v>
       </c>
@@ -2382,7 +2382,7 @@
         <v>0.43303636000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" s="1">
         <v>900</v>
       </c>
@@ -2402,7 +2402,7 @@
         <v>0.4390212</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" s="1">
         <v>1050</v>
       </c>
@@ -2422,7 +2422,7 @@
         <v>0.41385516999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" s="1">
         <v>1200</v>
       </c>
@@ -2442,7 +2442,7 @@
         <v>0.4139448</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" s="1">
         <v>1350</v>
       </c>
@@ -2462,7 +2462,7 @@
         <v>0.40282615999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" s="1">
         <v>1500</v>
       </c>
@@ -2482,7 +2482,7 @@
         <v>0.38751210000000003</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14" s="1">
         <v>1650</v>
       </c>
@@ -2502,7 +2502,7 @@
         <v>0.39523360000000002</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15" s="1">
         <v>1800</v>
       </c>
@@ -2522,7 +2522,7 @@
         <v>0.37737556999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16" s="1">
         <v>1950</v>
       </c>
@@ -2542,7 +2542,7 @@
         <v>0.38764710000000002</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17" s="1">
         <v>2100</v>
       </c>
@@ -2562,7 +2562,7 @@
         <v>0.41194984000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18" s="1">
         <v>2250</v>
       </c>
@@ -2582,7 +2582,7 @@
         <v>0.3760194</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19" s="1">
         <v>2400</v>
       </c>
@@ -2602,7 +2602,7 @@
         <v>0.37707287</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A20" s="1">
         <v>2550</v>
       </c>
@@ -2622,7 +2622,7 @@
         <v>0.38703108000000003</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A21" s="1">
         <v>2700</v>
       </c>

</xml_diff>

<commit_message>
selfie2anime was ich so geschafft habe
</commit_message>
<xml_diff>
--- a/Final_Project/Material_for_Documentation/Components of the Generator loss.xlsx
+++ b/Final_Project/Material_for_Documentation/Components of the Generator loss.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7febc520ade5fca9/Master_Cognitive_Computing/1_Semester/IANN_group30/Final_project/Material_for_Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F39A294-4FFD-4FF0-BCE3-4B29BB57511E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{4F39A294-4FFD-4FF0-BCE3-4B29BB57511E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{0DD87913-3B69-4D03-B6BE-6C01A59DC741}"/>
   <bookViews>
-    <workbookView xWindow="705" yWindow="705" windowWidth="16875" windowHeight="10523" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="705" yWindow="705" windowWidth="16875" windowHeight="10523" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="apple2orange" sheetId="2" r:id="rId1"/>
+    <sheet name="monet2photo" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="Generator_A_to_B_Losses" localSheetId="0">Tabelle1!$B$3:$F$21</definedName>
+    <definedName name="Generator_A_to_B_Losses" localSheetId="0">apple2orange!$B$3:$F$21</definedName>
+    <definedName name="Generator_A_to_B_Losses" localSheetId="1">monet2photo!$B$3:$F$21</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -40,11 +42,22 @@
       </textFields>
     </textPr>
   </connection>
+  <connection id="2" xr16:uid="{51068916-02D9-4756-B5C0-8D4FF11B46C2}" name="Generator_A_to_B_Losses1" type="6" refreshedVersion="6" background="1" saveData="1">
+    <textPr fileType="dos" sourceFile="C:\Users\Fabian\Desktop\Cognitive Computing Studium\Courses first semester\Implementing ANNs with TensorFlow\IANN_group30\Final_Project\Training_Results\Monet2Photo\Classical_Cycle_GAN\Generator_A_to_B_Losses.csv" decimal="," thousands="." tab="0" comma="1">
+      <textFields count="5">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="8">
   <si>
     <t>Adversarial loss</t>
   </si>
@@ -65,6 +78,9 @@
   </si>
   <si>
     <t>Monet2Photo: Classical Cycle GAN - Generator A to B training losses</t>
+  </si>
+  <si>
+    <t>Apple2Orange: Classical Cycle GAN - Generator A to B training losses</t>
   </si>
 </sst>
 </file>
@@ -258,7 +274,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Tabelle1!$A$4:$A$21</c:f>
+              <c:f>apple2orange!$A$4:$A$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
@@ -321,7 +337,1217 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Tabelle1!$B$4:$B$21</c:f>
+              <c:f>apple2orange!$B$4:$B$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>0.34111643000000003</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.31951722999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.47269707999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.59473056000000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.67166740000000003</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.61658513999999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.69666450000000002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.69061669999999997</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.66876303999999998</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.69713369999999997</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.69563070000000005</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.66580945000000002</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.64894706000000002</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.65795150000000002</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.73725980000000002</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.68093409999999999</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.64982430000000002</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.58375410000000005</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-C841-48D2-9CAD-79A5805C2F1A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Identity loss</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>apple2orange!$A$4:$A$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1050</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1200</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1350</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1650</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1800</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1950</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2100</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2250</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2400</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2550</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2700</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>apple2orange!$C$4:$C$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>0.41393626</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.36079642000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.34810447999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.33042919999999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.313249</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.31892189999999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.30673808000000002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.28647685000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.2926512</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.29481607999999998</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.31510177</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.27635077000000002</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.27669104999999999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.27750733</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.27101523</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.28645572000000002</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.26399400000000001</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.27607377999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-C841-48D2-9CAD-79A5805C2F1A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Forward loss</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>apple2orange!$A$4:$A$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1050</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1200</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1350</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1650</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1800</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1950</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2100</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2250</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2400</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2550</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2700</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>apple2orange!$D$4:$D$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>0.39641493999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.3408892</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.32116377000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.30232829999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.28562626000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.30692288000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.29923967000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.28132770000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.27199210000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.28219664</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.27228698000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.26975747999999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.24908847000000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.25828810000000002</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.26118322999999999</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.26235776999999999</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.25758170000000002</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.24504939000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-C841-48D2-9CAD-79A5805C2F1A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>Backward loss</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>apple2orange!$A$4:$A$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1050</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1200</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1350</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1650</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1800</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1950</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2100</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2250</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2400</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2550</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2700</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>apple2orange!$E$4:$E$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>0.42787882999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.36351559999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.3510453</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.33334416</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.32054456999999997</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.32069611999999997</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.30963624000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.29068031999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.29386064000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.29906981999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.31570290000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.27785992999999998</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.28191127999999999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.27774115999999999</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.27581716000000001</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.28971164999999999</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.27087489999999997</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.27901073999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-C841-48D2-9CAD-79A5805C2F1A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>Overall loss</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>apple2orange!$A$4:$A$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1050</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1200</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1350</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1650</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1800</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1950</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2100</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2250</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2400</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2550</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2700</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>apple2orange!$F$4:$F$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>0.66585857000000004</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.57297164</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.55845670000000003</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.53772489999999995</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.51872620000000003</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.53046159999999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.51994467</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.49019249999999998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.48690918</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.49899247000000002</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.50943989999999995</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.47023369999999998</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.45889990000000003</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.46286142000000002</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.46639617999999999</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.47711910000000002</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.45339742</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.45029530000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-C841-48D2-9CAD-79A5805C2F1A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1419001984"/>
+        <c:axId val="1418985760"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1419001984"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="2800"/>
+          <c:min val="100"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1200" b="1">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>Training step</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.38064004841860521"/>
+              <c:y val="0.93182221328424331"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1418985760"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1418985760"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="0.8"/>
+          <c:min val="0.1"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1200" b="1">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>Loss</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="8.0774577835304832E-3"/>
+              <c:y val="0.45682466263426308"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1419001984"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.82124141588465827"/>
+          <c:y val="0.39788015201439703"/>
+          <c:w val="0.17737898344898667"/>
+          <c:h val="0.29605293689958695"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1"/>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1600" b="1">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Components</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1600" b="1" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t> of the</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1600" b="1">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t> Generator loss</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="8.6136728628099568E-2"/>
+          <c:y val="0.11097257243630401"/>
+          <c:w val="0.73672787904936532"/>
+          <c:h val="0.76457363261812317"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Adversarial loss</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="FFC000"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>monet2photo!$A$4:$A$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1050</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1200</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1350</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1650</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1800</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1950</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2100</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2250</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2400</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2550</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2700</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>monet2photo!$B$4:$B$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
@@ -409,7 +1635,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Tabelle1!$A$4:$A$21</c:f>
+              <c:f>monet2photo!$A$4:$A$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
@@ -472,7 +1698,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Tabelle1!$C$4:$C$21</c:f>
+              <c:f>monet2photo!$C$4:$C$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
@@ -560,7 +1786,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Tabelle1!$A$4:$A$21</c:f>
+              <c:f>monet2photo!$A$4:$A$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
@@ -623,7 +1849,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Tabelle1!$D$4:$D$21</c:f>
+              <c:f>monet2photo!$D$4:$D$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
@@ -711,7 +1937,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Tabelle1!$A$4:$A$21</c:f>
+              <c:f>monet2photo!$A$4:$A$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
@@ -774,7 +2000,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Tabelle1!$E$4:$E$21</c:f>
+              <c:f>monet2photo!$E$4:$E$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
@@ -862,7 +2088,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Tabelle1!$A$4:$A$21</c:f>
+              <c:f>monet2photo!$A$4:$A$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
@@ -925,7 +2151,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Tabelle1!$F$4:$F$21</c:f>
+              <c:f>monet2photo!$F$4:$F$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
@@ -1383,6 +2609,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -1899,7 +3165,566 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>22860</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>601980</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Diagramm 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{04118F76-AE7D-4327-9625-B059A97EA7B6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -1941,6 +3766,10 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="Generator_A_to_B_Losses" connectionId="2" xr16:uid="{93DF0475-7538-4B87-B4E1-D8F1008E3251}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="Generator_A_to_B_Losses" connectionId="1" xr16:uid="{00000000-0016-0000-0000-000000000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
@@ -2240,11 +4069,421 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F22A03B5-13BF-4496-8409-089736363592}">
+  <dimension ref="A1:F21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="L26" sqref="L26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="2" max="2" width="13.53125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.53125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.46484375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="2"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A4" s="1">
+        <v>150</v>
+      </c>
+      <c r="B4">
+        <v>0.34111643000000003</v>
+      </c>
+      <c r="C4">
+        <v>0.41393626</v>
+      </c>
+      <c r="D4">
+        <v>0.39641493999999999</v>
+      </c>
+      <c r="E4">
+        <v>0.42787882999999999</v>
+      </c>
+      <c r="F4">
+        <v>0.66585857000000004</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A5" s="1">
+        <v>300</v>
+      </c>
+      <c r="B5">
+        <v>0.31951722999999999</v>
+      </c>
+      <c r="C5">
+        <v>0.36079642000000001</v>
+      </c>
+      <c r="D5">
+        <v>0.3408892</v>
+      </c>
+      <c r="E5">
+        <v>0.36351559999999999</v>
+      </c>
+      <c r="F5">
+        <v>0.57297164</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A6" s="1">
+        <v>450</v>
+      </c>
+      <c r="B6">
+        <v>0.47269707999999999</v>
+      </c>
+      <c r="C6">
+        <v>0.34810447999999999</v>
+      </c>
+      <c r="D6">
+        <v>0.32116377000000002</v>
+      </c>
+      <c r="E6">
+        <v>0.3510453</v>
+      </c>
+      <c r="F6">
+        <v>0.55845670000000003</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A7" s="1">
+        <v>600</v>
+      </c>
+      <c r="B7">
+        <v>0.59473056000000002</v>
+      </c>
+      <c r="C7">
+        <v>0.33042919999999998</v>
+      </c>
+      <c r="D7">
+        <v>0.30232829999999999</v>
+      </c>
+      <c r="E7">
+        <v>0.33334416</v>
+      </c>
+      <c r="F7">
+        <v>0.53772489999999995</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A8" s="1">
+        <v>750</v>
+      </c>
+      <c r="B8">
+        <v>0.67166740000000003</v>
+      </c>
+      <c r="C8">
+        <v>0.313249</v>
+      </c>
+      <c r="D8">
+        <v>0.28562626000000002</v>
+      </c>
+      <c r="E8">
+        <v>0.32054456999999997</v>
+      </c>
+      <c r="F8">
+        <v>0.51872620000000003</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A9" s="1">
+        <v>900</v>
+      </c>
+      <c r="B9">
+        <v>0.61658513999999998</v>
+      </c>
+      <c r="C9">
+        <v>0.31892189999999998</v>
+      </c>
+      <c r="D9">
+        <v>0.30692288000000001</v>
+      </c>
+      <c r="E9">
+        <v>0.32069611999999997</v>
+      </c>
+      <c r="F9">
+        <v>0.53046159999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A10" s="1">
+        <v>1050</v>
+      </c>
+      <c r="B10">
+        <v>0.69666450000000002</v>
+      </c>
+      <c r="C10">
+        <v>0.30673808000000002</v>
+      </c>
+      <c r="D10">
+        <v>0.29923967000000001</v>
+      </c>
+      <c r="E10">
+        <v>0.30963624000000001</v>
+      </c>
+      <c r="F10">
+        <v>0.51994467</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A11" s="1">
+        <v>1200</v>
+      </c>
+      <c r="B11">
+        <v>0.69061669999999997</v>
+      </c>
+      <c r="C11">
+        <v>0.28647685000000001</v>
+      </c>
+      <c r="D11">
+        <v>0.28132770000000001</v>
+      </c>
+      <c r="E11">
+        <v>0.29068031999999999</v>
+      </c>
+      <c r="F11">
+        <v>0.49019249999999998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A12" s="1">
+        <v>1350</v>
+      </c>
+      <c r="B12">
+        <v>0.66876303999999998</v>
+      </c>
+      <c r="C12">
+        <v>0.2926512</v>
+      </c>
+      <c r="D12">
+        <v>0.27199210000000001</v>
+      </c>
+      <c r="E12">
+        <v>0.29386064000000001</v>
+      </c>
+      <c r="F12">
+        <v>0.48690918</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A13" s="1">
+        <v>1500</v>
+      </c>
+      <c r="B13">
+        <v>0.69713369999999997</v>
+      </c>
+      <c r="C13">
+        <v>0.29481607999999998</v>
+      </c>
+      <c r="D13">
+        <v>0.28219664</v>
+      </c>
+      <c r="E13">
+        <v>0.29906981999999999</v>
+      </c>
+      <c r="F13">
+        <v>0.49899247000000002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A14" s="1">
+        <v>1650</v>
+      </c>
+      <c r="B14">
+        <v>0.69563070000000005</v>
+      </c>
+      <c r="C14">
+        <v>0.31510177</v>
+      </c>
+      <c r="D14">
+        <v>0.27228698000000001</v>
+      </c>
+      <c r="E14">
+        <v>0.31570290000000001</v>
+      </c>
+      <c r="F14">
+        <v>0.50943989999999995</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A15" s="1">
+        <v>1800</v>
+      </c>
+      <c r="B15">
+        <v>0.66580945000000002</v>
+      </c>
+      <c r="C15">
+        <v>0.27635077000000002</v>
+      </c>
+      <c r="D15">
+        <v>0.26975747999999999</v>
+      </c>
+      <c r="E15">
+        <v>0.27785992999999998</v>
+      </c>
+      <c r="F15">
+        <v>0.47023369999999998</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A16" s="1">
+        <v>1950</v>
+      </c>
+      <c r="B16">
+        <v>0.64894706000000002</v>
+      </c>
+      <c r="C16">
+        <v>0.27669104999999999</v>
+      </c>
+      <c r="D16">
+        <v>0.24908847000000001</v>
+      </c>
+      <c r="E16">
+        <v>0.28191127999999999</v>
+      </c>
+      <c r="F16">
+        <v>0.45889990000000003</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A17" s="1">
+        <v>2100</v>
+      </c>
+      <c r="B17">
+        <v>0.65795150000000002</v>
+      </c>
+      <c r="C17">
+        <v>0.27750733</v>
+      </c>
+      <c r="D17">
+        <v>0.25828810000000002</v>
+      </c>
+      <c r="E17">
+        <v>0.27774115999999999</v>
+      </c>
+      <c r="F17">
+        <v>0.46286142000000002</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A18" s="1">
+        <v>2250</v>
+      </c>
+      <c r="B18">
+        <v>0.73725980000000002</v>
+      </c>
+      <c r="C18">
+        <v>0.27101523</v>
+      </c>
+      <c r="D18">
+        <v>0.26118322999999999</v>
+      </c>
+      <c r="E18">
+        <v>0.27581716000000001</v>
+      </c>
+      <c r="F18">
+        <v>0.46639617999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A19" s="1">
+        <v>2400</v>
+      </c>
+      <c r="B19">
+        <v>0.68093409999999999</v>
+      </c>
+      <c r="C19">
+        <v>0.28645572000000002</v>
+      </c>
+      <c r="D19">
+        <v>0.26235776999999999</v>
+      </c>
+      <c r="E19">
+        <v>0.28971164999999999</v>
+      </c>
+      <c r="F19">
+        <v>0.47711910000000002</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A20" s="1">
+        <v>2550</v>
+      </c>
+      <c r="B20">
+        <v>0.64982430000000002</v>
+      </c>
+      <c r="C20">
+        <v>0.26399400000000001</v>
+      </c>
+      <c r="D20">
+        <v>0.25758170000000002</v>
+      </c>
+      <c r="E20">
+        <v>0.27087489999999997</v>
+      </c>
+      <c r="F20">
+        <v>0.45339742</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A21" s="1">
+        <v>2700</v>
+      </c>
+      <c r="B21">
+        <v>0.58375410000000005</v>
+      </c>
+      <c r="C21">
+        <v>0.27607377999999999</v>
+      </c>
+      <c r="D21">
+        <v>0.24504939000000001</v>
+      </c>
+      <c r="E21">
+        <v>0.27901073999999998</v>
+      </c>
+      <c r="F21">
+        <v>0.45029530000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>